<commit_message>
SDs added for fluoride conc
</commit_message>
<xml_diff>
--- a/Dehalogenation_colorimetric_assays/Fluoride Library screening 1 to 3 diluted.xlsx
+++ b/Dehalogenation_colorimetric_assays/Fluoride Library screening 1 to 3 diluted.xlsx
@@ -5,14 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eawag\userdata\felderfl\My Documents\GitHub\fluorinated_compounds_biotransformations\data\rawdata_Fluoride\20240113_fluoride screening\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\eawag\userdata\felderfl\My Documents\GitHub\gut_microbe_defluorination_paper\Dehalogenation_colorimetric_assays\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="9440" windowHeight="6920" activeTab="10"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="9440" windowHeight="6920"/>
   </bookViews>
   <sheets>
-    <sheet name="Data processing" sheetId="12" r:id="rId1"/>
+    <sheet name="Fluoride conc calculation" sheetId="12" r:id="rId1"/>
     <sheet name="P1.1" sheetId="1" r:id="rId2"/>
     <sheet name="P1.2" sheetId="2" r:id="rId3"/>
     <sheet name="P1.3" sheetId="3" r:id="rId4"/>
@@ -25,18 +25,18 @@
     <sheet name="Calibration 1to3 diluted" sheetId="13" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Data processing'!$B$84:$B$104</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Data processing'!$C$84:$C$104</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'Data processing'!$L$84:$L$104</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'Data processing'!$M$84:$M$104</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Data processing'!$D$84:$D$104</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Data processing'!$E$84:$E$104</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'Data processing'!$F$84:$F$104</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'Data processing'!$G$84:$G$104</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Data processing'!$H$84:$H$104</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Data processing'!$I$84:$I$104</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Data processing'!$J$84:$J$104</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Data processing'!$K$84:$K$104</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Fluoride conc calculation'!$B$84:$B$104</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Fluoride conc calculation'!$C$84:$C$104</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'Fluoride conc calculation'!$L$84:$L$104</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'Fluoride conc calculation'!$M$84:$M$104</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Fluoride conc calculation'!$D$84:$D$104</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Fluoride conc calculation'!$E$84:$E$104</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'Fluoride conc calculation'!$F$84:$F$104</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'Fluoride conc calculation'!$G$84:$G$104</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'Fluoride conc calculation'!$H$84:$H$104</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'Fluoride conc calculation'!$I$84:$I$104</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'Fluoride conc calculation'!$J$84:$J$104</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'Fluoride conc calculation'!$K$84:$K$104</definedName>
     <definedName name="MethodPointer1" localSheetId="10">-45104688</definedName>
     <definedName name="MethodPointer1">-379138160</definedName>
     <definedName name="MethodPointer2" localSheetId="10">683</definedName>
@@ -1110,6 +1110,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1128,10 +1132,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1351,7 +1351,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'Data processing'!$J$32:$O$32</c:f>
+                <c:f>'Fluoride conc calculation'!$J$32:$O$32</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
@@ -1378,7 +1378,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'Data processing'!$J$32:$O$32</c:f>
+                <c:f>'Fluoride conc calculation'!$J$32:$O$32</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="6"/>
@@ -1419,7 +1419,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'Data processing'!$J$29:$O$29</c:f>
+              <c:f>'Fluoride conc calculation'!$J$29:$O$29</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1446,7 +1446,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Data processing'!$J$30:$O$30</c:f>
+              <c:f>'Fluoride conc calculation'!$J$30:$O$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -3363,8 +3363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE118"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -14157,7 +14157,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="111" t="s">
+      <c r="B41" s="113" t="s">
         <v>25</v>
       </c>
       <c r="C41" s="63">
@@ -14201,7 +14201,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="112"/>
+      <c r="B42" s="114"/>
       <c r="C42" s="68">
         <v>0.45300000000000001</v>
       </c>
@@ -14243,7 +14243,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="112"/>
+      <c r="B43" s="114"/>
       <c r="C43" s="67">
         <v>0.67300000000000004</v>
       </c>
@@ -14285,7 +14285,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="112"/>
+      <c r="B44" s="114"/>
       <c r="C44" s="69">
         <v>0.54500000000000004</v>
       </c>
@@ -14327,7 +14327,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="113"/>
+      <c r="B45" s="115"/>
       <c r="C45" s="77">
         <v>0.60299999999999998</v>
       </c>
@@ -14369,7 +14369,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="111" t="s">
+      <c r="B46" s="113" t="s">
         <v>39</v>
       </c>
       <c r="C46" s="59">
@@ -14413,7 +14413,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="112"/>
+      <c r="B47" s="114"/>
       <c r="C47" s="68">
         <v>0.45100000000000001</v>
       </c>
@@ -14455,7 +14455,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="112"/>
+      <c r="B48" s="114"/>
       <c r="C48" s="66">
         <v>0.66700000000000004</v>
       </c>
@@ -14497,7 +14497,7 @@
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="112"/>
+      <c r="B49" s="114"/>
       <c r="C49" s="69">
         <v>0.54500000000000004</v>
       </c>
@@ -14539,7 +14539,7 @@
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="113"/>
+      <c r="B50" s="115"/>
       <c r="C50" s="80">
         <v>0.623</v>
       </c>
@@ -14581,7 +14581,7 @@
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="111" t="s">
+      <c r="B51" s="113" t="s">
         <v>52</v>
       </c>
       <c r="C51" s="62">
@@ -14625,7 +14625,7 @@
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B52" s="112"/>
+      <c r="B52" s="114"/>
       <c r="C52" s="70">
         <v>0.47199999999999998</v>
       </c>
@@ -14667,7 +14667,7 @@
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="112"/>
+      <c r="B53" s="114"/>
       <c r="C53" s="72">
         <v>0.71699999999999997</v>
       </c>
@@ -14709,7 +14709,7 @@
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="112"/>
+      <c r="B54" s="114"/>
       <c r="C54" s="73">
         <v>0.56000000000000005</v>
       </c>
@@ -14751,7 +14751,7 @@
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="113"/>
+      <c r="B55" s="115"/>
       <c r="C55" s="76">
         <v>0.53100000000000003</v>
       </c>
@@ -14793,7 +14793,7 @@
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="111" t="s">
+      <c r="B56" s="113" t="s">
         <v>65</v>
       </c>
       <c r="C56" s="62">
@@ -14837,7 +14837,7 @@
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="112"/>
+      <c r="B57" s="114"/>
       <c r="C57" s="70">
         <v>0.47299999999999998</v>
       </c>
@@ -14879,7 +14879,7 @@
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="112"/>
+      <c r="B58" s="114"/>
       <c r="C58" s="73">
         <v>0.74299999999999999</v>
       </c>
@@ -14921,7 +14921,7 @@
       </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="112"/>
+      <c r="B59" s="114"/>
       <c r="C59" s="70">
         <v>0.55800000000000005</v>
       </c>
@@ -14963,7 +14963,7 @@
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="113"/>
+      <c r="B60" s="115"/>
       <c r="C60" s="95">
         <v>0.439</v>
       </c>
@@ -15005,7 +15005,7 @@
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="111" t="s">
+      <c r="B61" s="113" t="s">
         <v>78</v>
       </c>
       <c r="C61" s="61">
@@ -15049,7 +15049,7 @@
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="112"/>
+      <c r="B62" s="114"/>
       <c r="C62" s="84">
         <v>0.48199999999999998</v>
       </c>
@@ -15091,7 +15091,7 @@
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="112"/>
+      <c r="B63" s="114"/>
       <c r="C63" s="84">
         <v>0.75700000000000001</v>
       </c>
@@ -15133,7 +15133,7 @@
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="112"/>
+      <c r="B64" s="114"/>
       <c r="C64" s="85">
         <v>0.56499999999999995</v>
       </c>
@@ -15175,7 +15175,7 @@
       </c>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B65" s="113"/>
+      <c r="B65" s="115"/>
       <c r="C65" s="95">
         <v>0.42699999999999999</v>
       </c>
@@ -15217,7 +15217,7 @@
       </c>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B66" s="111" t="s">
+      <c r="B66" s="113" t="s">
         <v>91</v>
       </c>
       <c r="C66" s="97">
@@ -15261,7 +15261,7 @@
       </c>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B67" s="112"/>
+      <c r="B67" s="114"/>
       <c r="C67" s="75">
         <v>0.43</v>
       </c>
@@ -15303,7 +15303,7 @@
       </c>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="112"/>
+      <c r="B68" s="114"/>
       <c r="C68" s="67">
         <v>0.67700000000000005</v>
       </c>
@@ -15345,7 +15345,7 @@
       </c>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="112"/>
+      <c r="B69" s="114"/>
       <c r="C69" s="69">
         <v>0.54600000000000004</v>
       </c>
@@ -15387,7 +15387,7 @@
       </c>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="113"/>
+      <c r="B70" s="115"/>
       <c r="C70" s="78">
         <v>0.51100000000000001</v>
       </c>
@@ -15429,7 +15429,7 @@
       </c>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B71" s="111" t="s">
+      <c r="B71" s="113" t="s">
         <v>104</v>
       </c>
       <c r="C71" s="96">
@@ -15473,7 +15473,7 @@
       </c>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="112"/>
+      <c r="B72" s="114"/>
       <c r="C72" s="74">
         <v>0.42299999999999999</v>
       </c>
@@ -15515,7 +15515,7 @@
       </c>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="112"/>
+      <c r="B73" s="114"/>
       <c r="C73" s="66">
         <v>0.66600000000000004</v>
       </c>
@@ -15557,7 +15557,7 @@
       </c>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="112"/>
+      <c r="B74" s="114"/>
       <c r="C74" s="75">
         <v>0.53700000000000003</v>
       </c>
@@ -15599,7 +15599,7 @@
       </c>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="113"/>
+      <c r="B75" s="115"/>
       <c r="C75" s="78">
         <v>0.502</v>
       </c>
@@ -15641,7 +15641,7 @@
       </c>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B76" s="111" t="s">
+      <c r="B76" s="113" t="s">
         <v>117</v>
       </c>
       <c r="C76" s="97">
@@ -15685,7 +15685,7 @@
       </c>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B77" s="112"/>
+      <c r="B77" s="114"/>
       <c r="C77" s="75">
         <v>0.42699999999999999</v>
       </c>
@@ -15727,7 +15727,7 @@
       </c>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="112"/>
+      <c r="B78" s="114"/>
       <c r="C78" s="67">
         <v>0.67500000000000004</v>
       </c>
@@ -15769,7 +15769,7 @@
       </c>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="112"/>
+      <c r="B79" s="114"/>
       <c r="C79" s="67">
         <v>0.54400000000000004</v>
       </c>
@@ -15811,7 +15811,7 @@
       </c>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="113"/>
+      <c r="B80" s="115"/>
       <c r="C80" s="78">
         <v>0.50600000000000001</v>
       </c>
@@ -17672,7 +17672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
@@ -17727,7 +17727,7 @@
       <c r="A8" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="115">
+      <c r="B8" s="109">
         <v>0.63942129629629629</v>
       </c>
     </row>
@@ -17883,7 +17883,7 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B29" s="111" t="s">
+      <c r="B29" s="113" t="s">
         <v>25</v>
       </c>
       <c r="C29" s="90">
@@ -17927,7 +17927,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B30" s="112"/>
+      <c r="B30" s="114"/>
       <c r="C30" s="86">
         <v>0.71399999999999997</v>
       </c>
@@ -17969,7 +17969,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B31" s="112"/>
+      <c r="B31" s="114"/>
       <c r="C31" s="87">
         <v>0.48699999999999999</v>
       </c>
@@ -18011,7 +18011,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B32" s="112"/>
+      <c r="B32" s="114"/>
       <c r="C32" s="87">
         <v>0.57599999999999996</v>
       </c>
@@ -18053,7 +18053,7 @@
       </c>
     </row>
     <row r="33" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="113"/>
+      <c r="B33" s="115"/>
       <c r="C33" s="81">
         <v>0.45</v>
       </c>
@@ -18095,7 +18095,7 @@
       </c>
     </row>
     <row r="34" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="111" t="s">
+      <c r="B34" s="113" t="s">
         <v>39</v>
       </c>
       <c r="C34" s="90">
@@ -18139,7 +18139,7 @@
       </c>
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B35" s="112"/>
+      <c r="B35" s="114"/>
       <c r="C35" s="86">
         <v>0.72699999999999998</v>
       </c>
@@ -18181,7 +18181,7 @@
       </c>
     </row>
     <row r="36" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B36" s="112"/>
+      <c r="B36" s="114"/>
       <c r="C36" s="87">
         <v>0.502</v>
       </c>
@@ -18223,7 +18223,7 @@
       </c>
     </row>
     <row r="37" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B37" s="112"/>
+      <c r="B37" s="114"/>
       <c r="C37" s="87">
         <v>0.58799999999999997</v>
       </c>
@@ -18265,7 +18265,7 @@
       </c>
     </row>
     <row r="38" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B38" s="113"/>
+      <c r="B38" s="115"/>
       <c r="C38" s="81">
         <v>0.46899999999999997</v>
       </c>
@@ -18307,7 +18307,7 @@
       </c>
     </row>
     <row r="39" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B39" s="111" t="s">
+      <c r="B39" s="113" t="s">
         <v>52</v>
       </c>
       <c r="C39" s="94">
@@ -18351,7 +18351,7 @@
       </c>
     </row>
     <row r="40" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B40" s="112"/>
+      <c r="B40" s="114"/>
       <c r="C40" s="74">
         <v>5.0999999999999997E-2</v>
       </c>
@@ -18393,7 +18393,7 @@
       </c>
     </row>
     <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="112"/>
+      <c r="B41" s="114"/>
       <c r="C41" s="74">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -18435,7 +18435,7 @@
       </c>
     </row>
     <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="112"/>
+      <c r="B42" s="114"/>
       <c r="C42" s="74">
         <v>4.9000000000000002E-2</v>
       </c>
@@ -18477,7 +18477,7 @@
       </c>
     </row>
     <row r="43" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="113"/>
+      <c r="B43" s="115"/>
       <c r="C43" s="89">
         <v>9.0999999999999998E-2</v>
       </c>
@@ -18519,7 +18519,7 @@
       </c>
     </row>
     <row r="44" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="111" t="s">
+      <c r="B44" s="113" t="s">
         <v>65</v>
       </c>
       <c r="C44" s="94">
@@ -18563,7 +18563,7 @@
       </c>
     </row>
     <row r="45" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="112"/>
+      <c r="B45" s="114"/>
       <c r="C45" s="74">
         <v>5.1999999999999998E-2</v>
       </c>
@@ -18605,7 +18605,7 @@
       </c>
     </row>
     <row r="46" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="112"/>
+      <c r="B46" s="114"/>
       <c r="C46" s="74">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -18647,7 +18647,7 @@
       </c>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="112"/>
+      <c r="B47" s="114"/>
       <c r="C47" s="74">
         <v>0.05</v>
       </c>
@@ -18689,7 +18689,7 @@
       </c>
     </row>
     <row r="48" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="113"/>
+      <c r="B48" s="115"/>
       <c r="C48" s="89">
         <v>8.7999999999999995E-2</v>
       </c>
@@ -18731,7 +18731,7 @@
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="111" t="s">
+      <c r="B49" s="113" t="s">
         <v>78</v>
       </c>
       <c r="C49" s="94">
@@ -18775,7 +18775,7 @@
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="112"/>
+      <c r="B50" s="114"/>
       <c r="C50" s="74">
         <v>5.1999999999999998E-2</v>
       </c>
@@ -18817,7 +18817,7 @@
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="112"/>
+      <c r="B51" s="114"/>
       <c r="C51" s="74">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -18859,7 +18859,7 @@
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B52" s="112"/>
+      <c r="B52" s="114"/>
       <c r="C52" s="74">
         <v>4.9000000000000002E-2</v>
       </c>
@@ -18901,7 +18901,7 @@
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="113"/>
+      <c r="B53" s="115"/>
       <c r="C53" s="89">
         <v>8.8999999999999996E-2</v>
       </c>
@@ -18943,7 +18943,7 @@
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="111" t="s">
+      <c r="B54" s="113" t="s">
         <v>91</v>
       </c>
       <c r="C54" s="94">
@@ -18987,7 +18987,7 @@
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="112"/>
+      <c r="B55" s="114"/>
       <c r="C55" s="74">
         <v>5.1999999999999998E-2</v>
       </c>
@@ -19029,7 +19029,7 @@
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="112"/>
+      <c r="B56" s="114"/>
       <c r="C56" s="74">
         <v>6.4000000000000001E-2</v>
       </c>
@@ -19071,7 +19071,7 @@
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="112"/>
+      <c r="B57" s="114"/>
       <c r="C57" s="74">
         <v>0.05</v>
       </c>
@@ -19113,7 +19113,7 @@
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="113"/>
+      <c r="B58" s="115"/>
       <c r="C58" s="89">
         <v>8.7999999999999995E-2</v>
       </c>
@@ -19155,7 +19155,7 @@
       </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="111" t="s">
+      <c r="B59" s="113" t="s">
         <v>104</v>
       </c>
       <c r="C59" s="94">
@@ -19199,7 +19199,7 @@
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="112"/>
+      <c r="B60" s="114"/>
       <c r="C60" s="74">
         <v>5.1999999999999998E-2</v>
       </c>
@@ -19241,7 +19241,7 @@
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="112"/>
+      <c r="B61" s="114"/>
       <c r="C61" s="74">
         <v>6.5000000000000002E-2</v>
       </c>
@@ -19283,7 +19283,7 @@
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="112"/>
+      <c r="B62" s="114"/>
       <c r="C62" s="74">
         <v>0.05</v>
       </c>
@@ -19325,7 +19325,7 @@
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="113"/>
+      <c r="B63" s="115"/>
       <c r="C63" s="89">
         <v>9.0999999999999998E-2</v>
       </c>
@@ -19367,7 +19367,7 @@
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="111" t="s">
+      <c r="B64" s="113" t="s">
         <v>117</v>
       </c>
       <c r="C64" s="94">
@@ -19411,7 +19411,7 @@
       </c>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B65" s="112"/>
+      <c r="B65" s="114"/>
       <c r="C65" s="74">
         <v>5.1999999999999998E-2</v>
       </c>
@@ -19453,7 +19453,7 @@
       </c>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B66" s="112"/>
+      <c r="B66" s="114"/>
       <c r="C66" s="74">
         <v>6.5000000000000002E-2</v>
       </c>
@@ -19495,7 +19495,7 @@
       </c>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B67" s="112"/>
+      <c r="B67" s="114"/>
       <c r="C67" s="74">
         <v>0.05</v>
       </c>
@@ -19537,7 +19537,7 @@
       </c>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="113"/>
+      <c r="B68" s="115"/>
       <c r="C68" s="89">
         <v>9.0999999999999998E-2</v>
       </c>
@@ -19579,74 +19579,74 @@
       </c>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="C70" s="114">
+      <c r="C70" s="108">
         <v>0</v>
       </c>
-      <c r="D70" s="114">
+      <c r="D70" s="108">
         <v>8.3330000000000002</v>
       </c>
-      <c r="E70" s="114">
+      <c r="E70" s="108">
         <v>25</v>
       </c>
-      <c r="F70" s="114">
+      <c r="F70" s="108">
         <v>50</v>
       </c>
-      <c r="G70" s="114">
+      <c r="G70" s="108">
         <v>75</v>
       </c>
-      <c r="H70" s="114">
+      <c r="H70" s="108">
         <v>100</v>
       </c>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C71" s="101">
-        <f>C32/C29</f>
+        <f t="shared" ref="C71:H71" si="0">C32/C29</f>
         <v>0.94581280788177335</v>
       </c>
       <c r="D71" s="101">
-        <f>D32/D29</f>
+        <f t="shared" si="0"/>
         <v>1.0395683453237408</v>
       </c>
       <c r="E71" s="101">
-        <f>E32/E29</f>
+        <f t="shared" si="0"/>
         <v>1.2644444444444443</v>
       </c>
       <c r="F71" s="101">
-        <f>F32/F29</f>
+        <f t="shared" si="0"/>
         <v>1.6089385474860334</v>
       </c>
       <c r="G71" s="101">
-        <f>G32/G29</f>
+        <f t="shared" si="0"/>
         <v>1.8673139158576051</v>
       </c>
       <c r="H71" s="101">
-        <f>H32/H29</f>
+        <f t="shared" si="0"/>
         <v>2.0179211469534049</v>
       </c>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C72" s="101">
-        <f>C37/C34</f>
+        <f t="shared" ref="C72:H72" si="1">C37/C34</f>
         <v>0.96551724137931028</v>
       </c>
       <c r="D72" s="101">
-        <f>D37/D34</f>
+        <f t="shared" si="1"/>
         <v>1.0195729537366547</v>
       </c>
       <c r="E72" s="101">
-        <f>E37/E34</f>
+        <f t="shared" si="1"/>
         <v>1.2435344827586206</v>
       </c>
       <c r="F72" s="101">
-        <f>F37/F34</f>
+        <f t="shared" si="1"/>
         <v>1.6078431372549018</v>
       </c>
       <c r="G72" s="101">
-        <f>G37/G34</f>
+        <f t="shared" si="1"/>
         <v>1.9006622516556291</v>
       </c>
       <c r="H72" s="101">
-        <f>H37/H34</f>
+        <f t="shared" si="1"/>
         <v>2.0215827338129495</v>
       </c>
     </row>
@@ -20278,7 +20278,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="108" t="s">
+      <c r="B41" s="110" t="s">
         <v>25</v>
       </c>
       <c r="C41" s="9">
@@ -20322,7 +20322,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="109"/>
+      <c r="B42" s="111"/>
       <c r="C42" s="15">
         <v>0.45800000000000002</v>
       </c>
@@ -20364,7 +20364,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="109"/>
+      <c r="B43" s="111"/>
       <c r="C43" s="15">
         <v>0.68300000000000005</v>
       </c>
@@ -20406,7 +20406,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="109"/>
+      <c r="B44" s="111"/>
       <c r="C44" s="17">
         <v>0.54300000000000004</v>
       </c>
@@ -20448,7 +20448,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="110"/>
+      <c r="B45" s="112"/>
       <c r="C45" s="23">
         <v>0.56000000000000005</v>
       </c>
@@ -20490,7 +20490,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="108" t="s">
+      <c r="B46" s="110" t="s">
         <v>39</v>
       </c>
       <c r="C46" s="28">
@@ -20534,7 +20534,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="109"/>
+      <c r="B47" s="111"/>
       <c r="C47" s="19">
         <v>0.46800000000000003</v>
       </c>
@@ -20576,7 +20576,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="109"/>
+      <c r="B48" s="111"/>
       <c r="C48" s="16">
         <v>0.68100000000000005</v>
       </c>
@@ -20618,7 +20618,7 @@
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="109"/>
+      <c r="B49" s="111"/>
       <c r="C49" s="31">
         <v>0.55600000000000005</v>
       </c>
@@ -20660,7 +20660,7 @@
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="110"/>
+      <c r="B50" s="112"/>
       <c r="C50" s="27">
         <v>0.63600000000000001</v>
       </c>
@@ -20702,7 +20702,7 @@
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="108" t="s">
+      <c r="B51" s="110" t="s">
         <v>52</v>
       </c>
       <c r="C51" s="30">
@@ -20746,7 +20746,7 @@
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B52" s="109"/>
+      <c r="B52" s="111"/>
       <c r="C52" s="20">
         <v>0.47799999999999998</v>
       </c>
@@ -20788,7 +20788,7 @@
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="109"/>
+      <c r="B53" s="111"/>
       <c r="C53" s="20">
         <v>0.749</v>
       </c>
@@ -20830,7 +20830,7 @@
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="109"/>
+      <c r="B54" s="111"/>
       <c r="C54" s="35">
         <v>0.55900000000000005</v>
       </c>
@@ -20872,7 +20872,7 @@
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="110"/>
+      <c r="B55" s="112"/>
       <c r="C55" s="44">
         <v>0.42799999999999999</v>
       </c>
@@ -20914,7 +20914,7 @@
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="108" t="s">
+      <c r="B56" s="110" t="s">
         <v>65</v>
       </c>
       <c r="C56" s="28">
@@ -20958,7 +20958,7 @@
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="109"/>
+      <c r="B57" s="111"/>
       <c r="C57" s="22">
         <v>0.47199999999999998</v>
       </c>
@@ -21000,7 +21000,7 @@
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="109"/>
+      <c r="B58" s="111"/>
       <c r="C58" s="22">
         <v>0.72499999999999998</v>
       </c>
@@ -21042,7 +21042,7 @@
       </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="109"/>
+      <c r="B59" s="111"/>
       <c r="C59" s="31">
         <v>0.55700000000000005</v>
       </c>
@@ -21084,7 +21084,7 @@
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="110"/>
+      <c r="B60" s="112"/>
       <c r="C60" s="25">
         <v>0.49299999999999999</v>
       </c>
@@ -21126,7 +21126,7 @@
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="108" t="s">
+      <c r="B61" s="110" t="s">
         <v>78</v>
       </c>
       <c r="C61" s="29">
@@ -21170,7 +21170,7 @@
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="109"/>
+      <c r="B62" s="111"/>
       <c r="C62" s="34">
         <v>0.47499999999999998</v>
       </c>
@@ -21212,7 +21212,7 @@
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="109"/>
+      <c r="B63" s="111"/>
       <c r="C63" s="34">
         <v>0.73199999999999998</v>
       </c>
@@ -21254,7 +21254,7 @@
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="109"/>
+      <c r="B64" s="111"/>
       <c r="C64" s="35">
         <v>0.56100000000000005</v>
       </c>
@@ -21296,7 +21296,7 @@
       </c>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B65" s="110"/>
+      <c r="B65" s="112"/>
       <c r="C65" s="25">
         <v>0.49</v>
       </c>
@@ -21338,7 +21338,7 @@
       </c>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B66" s="108" t="s">
+      <c r="B66" s="110" t="s">
         <v>91</v>
       </c>
       <c r="C66" s="14">
@@ -21382,7 +21382,7 @@
       </c>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B67" s="109"/>
+      <c r="B67" s="111"/>
       <c r="C67" s="32">
         <v>0.48799999999999999</v>
       </c>
@@ -21424,7 +21424,7 @@
       </c>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="109"/>
+      <c r="B68" s="111"/>
       <c r="C68" s="32">
         <v>0.77900000000000003</v>
       </c>
@@ -21466,7 +21466,7 @@
       </c>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="109"/>
+      <c r="B69" s="111"/>
       <c r="C69" s="32">
         <v>0.56200000000000006</v>
       </c>
@@ -21508,7 +21508,7 @@
       </c>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="110"/>
+      <c r="B70" s="112"/>
       <c r="C70" s="47">
         <v>0.35399999999999998</v>
       </c>
@@ -21550,7 +21550,7 @@
       </c>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B71" s="108" t="s">
+      <c r="B71" s="110" t="s">
         <v>104</v>
       </c>
       <c r="C71" s="11">
@@ -21594,7 +21594,7 @@
       </c>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="109"/>
+      <c r="B72" s="111"/>
       <c r="C72" s="17">
         <v>0.46300000000000002</v>
       </c>
@@ -21636,7 +21636,7 @@
       </c>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="109"/>
+      <c r="B73" s="111"/>
       <c r="C73" s="16">
         <v>0.67400000000000004</v>
       </c>
@@ -21678,7 +21678,7 @@
       </c>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="109"/>
+      <c r="B74" s="111"/>
       <c r="C74" s="20">
         <v>0.55300000000000005</v>
       </c>
@@ -21720,7 +21720,7 @@
       </c>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="110"/>
+      <c r="B75" s="112"/>
       <c r="C75" s="27">
         <v>0.63900000000000001</v>
       </c>
@@ -21762,7 +21762,7 @@
       </c>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B76" s="108" t="s">
+      <c r="B76" s="110" t="s">
         <v>117</v>
       </c>
       <c r="C76" s="30">
@@ -21806,7 +21806,7 @@
       </c>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B77" s="109"/>
+      <c r="B77" s="111"/>
       <c r="C77" s="34">
         <v>0.47499999999999998</v>
       </c>
@@ -21848,7 +21848,7 @@
       </c>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="109"/>
+      <c r="B78" s="111"/>
       <c r="C78" s="34">
         <v>0.73</v>
       </c>
@@ -21890,7 +21890,7 @@
       </c>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="109"/>
+      <c r="B79" s="111"/>
       <c r="C79" s="31">
         <v>0.55800000000000005</v>
       </c>
@@ -21932,7 +21932,7 @@
       </c>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="110"/>
+      <c r="B80" s="112"/>
       <c r="C80" s="45">
         <v>0.48399999999999999</v>
       </c>
@@ -23065,7 +23065,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="111" t="s">
+      <c r="B41" s="113" t="s">
         <v>25</v>
       </c>
       <c r="C41" s="58">
@@ -23109,7 +23109,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="112"/>
+      <c r="B42" s="114"/>
       <c r="C42" s="66">
         <v>0.45500000000000002</v>
       </c>
@@ -23151,7 +23151,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="112"/>
+      <c r="B43" s="114"/>
       <c r="C43" s="66">
         <v>0.68300000000000005</v>
       </c>
@@ -23193,7 +23193,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="112"/>
+      <c r="B44" s="114"/>
       <c r="C44" s="74">
         <v>0.53700000000000003</v>
       </c>
@@ -23235,7 +23235,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="113"/>
+      <c r="B45" s="115"/>
       <c r="C45" s="76">
         <v>0.52800000000000002</v>
       </c>
@@ -23277,7 +23277,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="111" t="s">
+      <c r="B46" s="113" t="s">
         <v>39</v>
       </c>
       <c r="C46" s="64">
@@ -23321,7 +23321,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="112"/>
+      <c r="B47" s="114"/>
       <c r="C47" s="71">
         <v>0.46600000000000003</v>
       </c>
@@ -23363,7 +23363,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="112"/>
+      <c r="B48" s="114"/>
       <c r="C48" s="66">
         <v>0.67700000000000005</v>
       </c>
@@ -23405,7 +23405,7 @@
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="112"/>
+      <c r="B49" s="114"/>
       <c r="C49" s="70">
         <v>0.55300000000000005</v>
       </c>
@@ -23447,7 +23447,7 @@
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="113"/>
+      <c r="B50" s="115"/>
       <c r="C50" s="81">
         <v>0.63300000000000001</v>
       </c>
@@ -23489,7 +23489,7 @@
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="111" t="s">
+      <c r="B51" s="113" t="s">
         <v>52</v>
       </c>
       <c r="C51" s="65">
@@ -23533,7 +23533,7 @@
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B52" s="112"/>
+      <c r="B52" s="114"/>
       <c r="C52" s="70">
         <v>0.47299999999999998</v>
       </c>
@@ -23575,7 +23575,7 @@
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="112"/>
+      <c r="B53" s="114"/>
       <c r="C53" s="72">
         <v>0.72799999999999998</v>
       </c>
@@ -23617,7 +23617,7 @@
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="112"/>
+      <c r="B54" s="114"/>
       <c r="C54" s="73">
         <v>0.55500000000000005</v>
       </c>
@@ -23659,7 +23659,7 @@
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="113"/>
+      <c r="B55" s="115"/>
       <c r="C55" s="88">
         <v>0.47199999999999998</v>
       </c>
@@ -23701,7 +23701,7 @@
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="111" t="s">
+      <c r="B56" s="113" t="s">
         <v>65</v>
       </c>
       <c r="C56" s="64">
@@ -23745,7 +23745,7 @@
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="112"/>
+      <c r="B57" s="114"/>
       <c r="C57" s="71">
         <v>0.46899999999999997</v>
       </c>
@@ -23787,7 +23787,7 @@
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="112"/>
+      <c r="B58" s="114"/>
       <c r="C58" s="68">
         <v>0.71099999999999997</v>
       </c>
@@ -23829,7 +23829,7 @@
       </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="112"/>
+      <c r="B59" s="114"/>
       <c r="C59" s="84">
         <v>0.55800000000000005</v>
       </c>
@@ -23871,7 +23871,7 @@
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="113"/>
+      <c r="B60" s="115"/>
       <c r="C60" s="76">
         <v>0.53700000000000003</v>
       </c>
@@ -23913,7 +23913,7 @@
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="111" t="s">
+      <c r="B61" s="113" t="s">
         <v>78</v>
       </c>
       <c r="C61" s="83">
@@ -23957,7 +23957,7 @@
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="112"/>
+      <c r="B62" s="114"/>
       <c r="C62" s="68">
         <v>0.46500000000000002</v>
       </c>
@@ -23999,7 +23999,7 @@
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="112"/>
+      <c r="B63" s="114"/>
       <c r="C63" s="68">
         <v>0.71699999999999997</v>
       </c>
@@ -24041,7 +24041,7 @@
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="112"/>
+      <c r="B64" s="114"/>
       <c r="C64" s="71">
         <v>0.55000000000000004</v>
       </c>
@@ -24083,7 +24083,7 @@
       </c>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B65" s="113"/>
+      <c r="B65" s="115"/>
       <c r="C65" s="88">
         <v>0.48599999999999999</v>
       </c>
@@ -24125,7 +24125,7 @@
       </c>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B66" s="111" t="s">
+      <c r="B66" s="113" t="s">
         <v>91</v>
       </c>
       <c r="C66" s="64">
@@ -24169,7 +24169,7 @@
       </c>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B67" s="112"/>
+      <c r="B67" s="114"/>
       <c r="C67" s="70">
         <v>0.47299999999999998</v>
       </c>
@@ -24211,7 +24211,7 @@
       </c>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="112"/>
+      <c r="B68" s="114"/>
       <c r="C68" s="73">
         <v>0.755</v>
       </c>
@@ -24253,7 +24253,7 @@
       </c>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="112"/>
+      <c r="B69" s="114"/>
       <c r="C69" s="70">
         <v>0.55500000000000005</v>
       </c>
@@ -24295,7 +24295,7 @@
       </c>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="113"/>
+      <c r="B70" s="115"/>
       <c r="C70" s="92">
         <v>0.38900000000000001</v>
       </c>
@@ -24337,7 +24337,7 @@
       </c>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B71" s="111" t="s">
+      <c r="B71" s="113" t="s">
         <v>104</v>
       </c>
       <c r="C71" s="60">
@@ -24381,7 +24381,7 @@
       </c>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="112"/>
+      <c r="B72" s="114"/>
       <c r="C72" s="74">
         <v>0.44800000000000001</v>
       </c>
@@ -24423,7 +24423,7 @@
       </c>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="112"/>
+      <c r="B73" s="114"/>
       <c r="C73" s="74">
         <v>0.65600000000000003</v>
       </c>
@@ -24465,7 +24465,7 @@
       </c>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="112"/>
+      <c r="B74" s="114"/>
       <c r="C74" s="74">
         <v>0.53800000000000003</v>
       </c>
@@ -24507,7 +24507,7 @@
       </c>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="113"/>
+      <c r="B75" s="115"/>
       <c r="C75" s="81">
         <v>0.623</v>
       </c>
@@ -24549,7 +24549,7 @@
       </c>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B76" s="111" t="s">
+      <c r="B76" s="113" t="s">
         <v>117</v>
       </c>
       <c r="C76" s="59">
@@ -24593,7 +24593,7 @@
       </c>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B77" s="112"/>
+      <c r="B77" s="114"/>
       <c r="C77" s="67">
         <v>0.46</v>
       </c>
@@ -24635,7 +24635,7 @@
       </c>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="112"/>
+      <c r="B78" s="114"/>
       <c r="C78" s="68">
         <v>0.71599999999999997</v>
       </c>
@@ -24677,7 +24677,7 @@
       </c>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="112"/>
+      <c r="B79" s="114"/>
       <c r="C79" s="67">
         <v>0.54300000000000004</v>
       </c>
@@ -24719,7 +24719,7 @@
       </c>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="113"/>
+      <c r="B80" s="115"/>
       <c r="C80" s="82">
         <v>0.45400000000000001</v>
       </c>
@@ -25851,7 +25851,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="111" t="s">
+      <c r="B41" s="113" t="s">
         <v>25</v>
       </c>
       <c r="C41" s="60">
@@ -25895,7 +25895,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="112"/>
+      <c r="B42" s="114"/>
       <c r="C42" s="66">
         <v>0.45100000000000001</v>
       </c>
@@ -25937,7 +25937,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="112"/>
+      <c r="B43" s="114"/>
       <c r="C43" s="66">
         <v>0.68</v>
       </c>
@@ -25979,7 +25979,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="112"/>
+      <c r="B44" s="114"/>
       <c r="C44" s="74">
         <v>0.54</v>
       </c>
@@ -26021,7 +26021,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="113"/>
+      <c r="B45" s="115"/>
       <c r="C45" s="79">
         <v>0.55700000000000005</v>
       </c>
@@ -26063,7 +26063,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="111" t="s">
+      <c r="B46" s="113" t="s">
         <v>39</v>
       </c>
       <c r="C46" s="63">
@@ -26107,7 +26107,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="112"/>
+      <c r="B47" s="114"/>
       <c r="C47" s="67">
         <v>0.45400000000000001</v>
       </c>
@@ -26149,7 +26149,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="112"/>
+      <c r="B48" s="114"/>
       <c r="C48" s="74">
         <v>0.66200000000000003</v>
       </c>
@@ -26191,7 +26191,7 @@
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="112"/>
+      <c r="B49" s="114"/>
       <c r="C49" s="66">
         <v>0.54400000000000004</v>
       </c>
@@ -26233,7 +26233,7 @@
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="113"/>
+      <c r="B50" s="115"/>
       <c r="C50" s="81">
         <v>0.63700000000000001</v>
       </c>
@@ -26275,7 +26275,7 @@
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="111" t="s">
+      <c r="B51" s="113" t="s">
         <v>52</v>
       </c>
       <c r="C51" s="64">
@@ -26319,7 +26319,7 @@
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B52" s="112"/>
+      <c r="B52" s="114"/>
       <c r="C52" s="70">
         <v>0.46700000000000003</v>
       </c>
@@ -26361,7 +26361,7 @@
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="112"/>
+      <c r="B53" s="114"/>
       <c r="C53" s="70">
         <v>0.74299999999999999</v>
       </c>
@@ -26403,7 +26403,7 @@
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="112"/>
+      <c r="B54" s="114"/>
       <c r="C54" s="68">
         <v>0.54900000000000004</v>
       </c>
@@ -26445,7 +26445,7 @@
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="113"/>
+      <c r="B55" s="115"/>
       <c r="C55" s="93">
         <v>0.39700000000000002</v>
       </c>
@@ -26487,7 +26487,7 @@
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="111" t="s">
+      <c r="B56" s="113" t="s">
         <v>65</v>
       </c>
       <c r="C56" s="83">
@@ -26531,7 +26531,7 @@
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="112"/>
+      <c r="B57" s="114"/>
       <c r="C57" s="71">
         <v>0.46200000000000002</v>
       </c>
@@ -26573,7 +26573,7 @@
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="112"/>
+      <c r="B58" s="114"/>
       <c r="C58" s="68">
         <v>0.70799999999999996</v>
       </c>
@@ -26615,7 +26615,7 @@
       </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="112"/>
+      <c r="B59" s="114"/>
       <c r="C59" s="72">
         <v>0.55300000000000005</v>
       </c>
@@ -26657,7 +26657,7 @@
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="113"/>
+      <c r="B60" s="115"/>
       <c r="C60" s="76">
         <v>0.52700000000000002</v>
       </c>
@@ -26699,7 +26699,7 @@
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="111" t="s">
+      <c r="B61" s="113" t="s">
         <v>78</v>
       </c>
       <c r="C61" s="63">
@@ -26743,7 +26743,7 @@
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="112"/>
+      <c r="B62" s="114"/>
       <c r="C62" s="69">
         <v>0.45900000000000002</v>
       </c>
@@ -26785,7 +26785,7 @@
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="112"/>
+      <c r="B63" s="114"/>
       <c r="C63" s="69">
         <v>0.70599999999999996</v>
       </c>
@@ -26827,7 +26827,7 @@
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="112"/>
+      <c r="B64" s="114"/>
       <c r="C64" s="68">
         <v>0.55100000000000005</v>
       </c>
@@ -26869,7 +26869,7 @@
       </c>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B65" s="113"/>
+      <c r="B65" s="115"/>
       <c r="C65" s="76">
         <v>0.52300000000000002</v>
       </c>
@@ -26911,7 +26911,7 @@
       </c>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B66" s="111" t="s">
+      <c r="B66" s="113" t="s">
         <v>91</v>
       </c>
       <c r="C66" s="83">
@@ -26955,7 +26955,7 @@
       </c>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B67" s="112"/>
+      <c r="B67" s="114"/>
       <c r="C67" s="72">
         <v>0.46600000000000003</v>
       </c>
@@ -26997,7 +26997,7 @@
       </c>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="112"/>
+      <c r="B68" s="114"/>
       <c r="C68" s="84">
         <v>0.75700000000000001</v>
       </c>
@@ -27039,7 +27039,7 @@
       </c>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="112"/>
+      <c r="B69" s="114"/>
       <c r="C69" s="71">
         <v>0.55300000000000005</v>
       </c>
@@ -27081,7 +27081,7 @@
       </c>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="113"/>
+      <c r="B70" s="115"/>
       <c r="C70" s="92">
         <v>0.374</v>
       </c>
@@ -27123,7 +27123,7 @@
       </c>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B71" s="111" t="s">
+      <c r="B71" s="113" t="s">
         <v>104</v>
       </c>
       <c r="C71" s="83">
@@ -27167,7 +27167,7 @@
       </c>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="112"/>
+      <c r="B72" s="114"/>
       <c r="C72" s="68">
         <v>0.45900000000000002</v>
       </c>
@@ -27209,7 +27209,7 @@
       </c>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="112"/>
+      <c r="B73" s="114"/>
       <c r="C73" s="75">
         <v>0.67200000000000004</v>
       </c>
@@ -27251,7 +27251,7 @@
       </c>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="112"/>
+      <c r="B74" s="114"/>
       <c r="C74" s="72">
         <v>0.55500000000000005</v>
       </c>
@@ -27293,7 +27293,7 @@
       </c>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="113"/>
+      <c r="B75" s="115"/>
       <c r="C75" s="81">
         <v>0.65400000000000003</v>
       </c>
@@ -27335,7 +27335,7 @@
       </c>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B76" s="111" t="s">
+      <c r="B76" s="113" t="s">
         <v>117</v>
       </c>
       <c r="C76" s="59">
@@ -27379,7 +27379,7 @@
       </c>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B77" s="112"/>
+      <c r="B77" s="114"/>
       <c r="C77" s="69">
         <v>0.45800000000000002</v>
       </c>
@@ -27421,7 +27421,7 @@
       </c>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="112"/>
+      <c r="B78" s="114"/>
       <c r="C78" s="68">
         <v>0.71399999999999997</v>
       </c>
@@ -27463,7 +27463,7 @@
       </c>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="112"/>
+      <c r="B79" s="114"/>
       <c r="C79" s="69">
         <v>0.54800000000000004</v>
       </c>
@@ -27505,7 +27505,7 @@
       </c>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="113"/>
+      <c r="B80" s="115"/>
       <c r="C80" s="88">
         <v>0.48899999999999999</v>
       </c>
@@ -29974,7 +29974,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="111" t="s">
+      <c r="B41" s="113" t="s">
         <v>25</v>
       </c>
       <c r="C41" s="63">
@@ -30018,7 +30018,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="112"/>
+      <c r="B42" s="114"/>
       <c r="C42" s="71">
         <v>0.47399999999999998</v>
       </c>
@@ -30060,7 +30060,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="112"/>
+      <c r="B43" s="114"/>
       <c r="C43" s="71">
         <v>0.72499999999999998</v>
       </c>
@@ -30102,7 +30102,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="112"/>
+      <c r="B44" s="114"/>
       <c r="C44" s="71">
         <v>0.55500000000000005</v>
       </c>
@@ -30144,7 +30144,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="113"/>
+      <c r="B45" s="115"/>
       <c r="C45" s="88">
         <v>0.48399999999999999</v>
       </c>
@@ -30186,7 +30186,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="111" t="s">
+      <c r="B46" s="113" t="s">
         <v>39</v>
       </c>
       <c r="C46" s="63">
@@ -30230,7 +30230,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="112"/>
+      <c r="B47" s="114"/>
       <c r="C47" s="71">
         <v>0.47499999999999998</v>
       </c>
@@ -30272,7 +30272,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="112"/>
+      <c r="B48" s="114"/>
       <c r="C48" s="72">
         <v>0.73599999999999999</v>
       </c>
@@ -30314,7 +30314,7 @@
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="112"/>
+      <c r="B49" s="114"/>
       <c r="C49" s="72">
         <v>0.55600000000000005</v>
       </c>
@@ -30356,7 +30356,7 @@
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="113"/>
+      <c r="B50" s="115"/>
       <c r="C50" s="82">
         <v>0.45</v>
       </c>
@@ -30398,7 +30398,7 @@
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="111" t="s">
+      <c r="B51" s="113" t="s">
         <v>52</v>
       </c>
       <c r="C51" s="90">
@@ -30442,7 +30442,7 @@
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B52" s="112"/>
+      <c r="B52" s="114"/>
       <c r="C52" s="87">
         <v>0.51700000000000002</v>
       </c>
@@ -30484,7 +30484,7 @@
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="112"/>
+      <c r="B53" s="114"/>
       <c r="C53" s="87">
         <v>0.82299999999999995</v>
       </c>
@@ -30526,7 +30526,7 @@
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="112"/>
+      <c r="B54" s="114"/>
       <c r="C54" s="86">
         <v>0.57899999999999996</v>
       </c>
@@ -30568,7 +30568,7 @@
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="113"/>
+      <c r="B55" s="115"/>
       <c r="C55" s="89">
         <v>0.29499999999999998</v>
       </c>
@@ -30610,7 +30610,7 @@
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="111" t="s">
+      <c r="B56" s="113" t="s">
         <v>65</v>
       </c>
       <c r="C56" s="64">
@@ -30654,7 +30654,7 @@
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="112"/>
+      <c r="B57" s="114"/>
       <c r="C57" s="70">
         <v>0.48499999999999999</v>
       </c>
@@ -30696,7 +30696,7 @@
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="112"/>
+      <c r="B58" s="114"/>
       <c r="C58" s="67">
         <v>0.69299999999999995</v>
       </c>
@@ -30738,7 +30738,7 @@
       </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="112"/>
+      <c r="B59" s="114"/>
       <c r="C59" s="73">
         <v>0.56499999999999995</v>
       </c>
@@ -30780,7 +30780,7 @@
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="113"/>
+      <c r="B60" s="115"/>
       <c r="C60" s="81">
         <v>0.63500000000000001</v>
       </c>
@@ -30822,7 +30822,7 @@
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="111" t="s">
+      <c r="B61" s="113" t="s">
         <v>78</v>
       </c>
       <c r="C61" s="58">
@@ -30866,7 +30866,7 @@
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="112"/>
+      <c r="B62" s="114"/>
       <c r="C62" s="69">
         <v>0.46</v>
       </c>
@@ -30908,7 +30908,7 @@
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="112"/>
+      <c r="B63" s="114"/>
       <c r="C63" s="66">
         <v>0.67500000000000004</v>
       </c>
@@ -30950,7 +30950,7 @@
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="112"/>
+      <c r="B64" s="114"/>
       <c r="C64" s="71">
         <v>0.55300000000000005</v>
       </c>
@@ -30992,7 +30992,7 @@
       </c>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B65" s="113"/>
+      <c r="B65" s="115"/>
       <c r="C65" s="81">
         <v>0.64</v>
       </c>
@@ -31034,7 +31034,7 @@
       </c>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B66" s="111" t="s">
+      <c r="B66" s="113" t="s">
         <v>91</v>
       </c>
       <c r="C66" s="83">
@@ -31078,7 +31078,7 @@
       </c>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B67" s="112"/>
+      <c r="B67" s="114"/>
       <c r="C67" s="71">
         <v>0.47599999999999998</v>
       </c>
@@ -31120,7 +31120,7 @@
       </c>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="112"/>
+      <c r="B68" s="114"/>
       <c r="C68" s="66">
         <v>0.68300000000000005</v>
       </c>
@@ -31162,7 +31162,7 @@
       </c>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="112"/>
+      <c r="B69" s="114"/>
       <c r="C69" s="72">
         <v>0.55600000000000005</v>
       </c>
@@ -31204,7 +31204,7 @@
       </c>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="113"/>
+      <c r="B70" s="115"/>
       <c r="C70" s="81">
         <v>0.627</v>
       </c>
@@ -31246,7 +31246,7 @@
       </c>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B71" s="111" t="s">
+      <c r="B71" s="113" t="s">
         <v>104</v>
       </c>
       <c r="C71" s="59">
@@ -31290,7 +31290,7 @@
       </c>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="112"/>
+      <c r="B72" s="114"/>
       <c r="C72" s="69">
         <v>0.46400000000000002</v>
       </c>
@@ -31332,7 +31332,7 @@
       </c>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="112"/>
+      <c r="B73" s="114"/>
       <c r="C73" s="66">
         <v>0.67600000000000005</v>
       </c>
@@ -31374,7 +31374,7 @@
       </c>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="112"/>
+      <c r="B74" s="114"/>
       <c r="C74" s="68">
         <v>0.55000000000000004</v>
       </c>
@@ -31416,7 +31416,7 @@
       </c>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="113"/>
+      <c r="B75" s="115"/>
       <c r="C75" s="80">
         <v>0.61699999999999999</v>
       </c>
@@ -31458,7 +31458,7 @@
       </c>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B76" s="111" t="s">
+      <c r="B76" s="113" t="s">
         <v>117</v>
       </c>
       <c r="C76" s="60">
@@ -31502,7 +31502,7 @@
       </c>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B77" s="112"/>
+      <c r="B77" s="114"/>
       <c r="C77" s="67">
         <v>0.45800000000000002</v>
       </c>
@@ -31544,7 +31544,7 @@
       </c>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="112"/>
+      <c r="B78" s="114"/>
       <c r="C78" s="75">
         <v>0.67100000000000004</v>
       </c>
@@ -31586,7 +31586,7 @@
       </c>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="112"/>
+      <c r="B79" s="114"/>
       <c r="C79" s="68">
         <v>0.55000000000000004</v>
       </c>
@@ -31628,7 +31628,7 @@
       </c>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="113"/>
+      <c r="B80" s="115"/>
       <c r="C80" s="81">
         <v>0.63600000000000001</v>
       </c>
@@ -34097,7 +34097,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="111" t="s">
+      <c r="B41" s="113" t="s">
         <v>25</v>
       </c>
       <c r="C41" s="60">
@@ -34141,7 +34141,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="112"/>
+      <c r="B42" s="114"/>
       <c r="C42" s="67">
         <v>0.45600000000000002</v>
       </c>
@@ -34183,7 +34183,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="112"/>
+      <c r="B43" s="114"/>
       <c r="C43" s="67">
         <v>0.68899999999999995</v>
       </c>
@@ -34225,7 +34225,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="112"/>
+      <c r="B44" s="114"/>
       <c r="C44" s="66">
         <v>0.53600000000000003</v>
       </c>
@@ -34267,7 +34267,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="113"/>
+      <c r="B45" s="115"/>
       <c r="C45" s="78">
         <v>0.502</v>
       </c>
@@ -34309,7 +34309,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="111" t="s">
+      <c r="B46" s="113" t="s">
         <v>39</v>
       </c>
       <c r="C46" s="58">
@@ -34353,7 +34353,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="112"/>
+      <c r="B47" s="114"/>
       <c r="C47" s="69">
         <v>0.46100000000000002</v>
       </c>
@@ -34395,7 +34395,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="112"/>
+      <c r="B48" s="114"/>
       <c r="C48" s="68">
         <v>0.70499999999999996</v>
       </c>
@@ -34437,7 +34437,7 @@
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="112"/>
+      <c r="B49" s="114"/>
       <c r="C49" s="69">
         <v>0.54400000000000004</v>
       </c>
@@ -34479,7 +34479,7 @@
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="113"/>
+      <c r="B50" s="115"/>
       <c r="C50" s="78">
         <v>0.49</v>
       </c>
@@ -34521,7 +34521,7 @@
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="111" t="s">
+      <c r="B51" s="113" t="s">
         <v>52</v>
       </c>
       <c r="C51" s="61">
@@ -34565,7 +34565,7 @@
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B52" s="112"/>
+      <c r="B52" s="114"/>
       <c r="C52" s="84">
         <v>0.49299999999999999</v>
       </c>
@@ -34607,7 +34607,7 @@
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="112"/>
+      <c r="B53" s="114"/>
       <c r="C53" s="86">
         <v>0.78800000000000003</v>
       </c>
@@ -34649,7 +34649,7 @@
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="112"/>
+      <c r="B54" s="114"/>
       <c r="C54" s="72">
         <v>0.55400000000000005</v>
       </c>
@@ -34691,7 +34691,7 @@
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="113"/>
+      <c r="B55" s="115"/>
       <c r="C55" s="89">
         <v>0.28399999999999997</v>
       </c>
@@ -34733,7 +34733,7 @@
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="111" t="s">
+      <c r="B56" s="113" t="s">
         <v>65</v>
       </c>
       <c r="C56" s="62">
@@ -34777,7 +34777,7 @@
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="112"/>
+      <c r="B57" s="114"/>
       <c r="C57" s="72">
         <v>0.47499999999999998</v>
       </c>
@@ -34819,7 +34819,7 @@
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="112"/>
+      <c r="B58" s="114"/>
       <c r="C58" s="66">
         <v>0.67800000000000005</v>
       </c>
@@ -34861,7 +34861,7 @@
       </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="112"/>
+      <c r="B59" s="114"/>
       <c r="C59" s="72">
         <v>0.55300000000000005</v>
       </c>
@@ -34903,7 +34903,7 @@
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="113"/>
+      <c r="B60" s="115"/>
       <c r="C60" s="81">
         <v>0.62</v>
       </c>
@@ -34945,7 +34945,7 @@
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="111" t="s">
+      <c r="B61" s="113" t="s">
         <v>78</v>
       </c>
       <c r="C61" s="97">
@@ -34989,7 +34989,7 @@
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="112"/>
+      <c r="B62" s="114"/>
       <c r="C62" s="75">
         <v>0.44500000000000001</v>
       </c>
@@ -35031,7 +35031,7 @@
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="112"/>
+      <c r="B63" s="114"/>
       <c r="C63" s="74">
         <v>0.65200000000000002</v>
       </c>
@@ -35073,7 +35073,7 @@
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="112"/>
+      <c r="B64" s="114"/>
       <c r="C64" s="75">
         <v>0.53500000000000003</v>
       </c>
@@ -35115,7 +35115,7 @@
       </c>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B65" s="113"/>
+      <c r="B65" s="115"/>
       <c r="C65" s="81">
         <v>0.623</v>
       </c>
@@ -35157,7 +35157,7 @@
       </c>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B66" s="111" t="s">
+      <c r="B66" s="113" t="s">
         <v>91</v>
       </c>
       <c r="C66" s="62">
@@ -35201,7 +35201,7 @@
       </c>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B67" s="112"/>
+      <c r="B67" s="114"/>
       <c r="C67" s="71">
         <v>0.47399999999999998</v>
       </c>
@@ -35243,7 +35243,7 @@
       </c>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="112"/>
+      <c r="B68" s="114"/>
       <c r="C68" s="66">
         <v>0.67400000000000004</v>
       </c>
@@ -35285,7 +35285,7 @@
       </c>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="112"/>
+      <c r="B69" s="114"/>
       <c r="C69" s="72">
         <v>0.55100000000000005</v>
       </c>
@@ -35327,7 +35327,7 @@
       </c>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="113"/>
+      <c r="B70" s="115"/>
       <c r="C70" s="81">
         <v>0.627</v>
       </c>
@@ -35369,7 +35369,7 @@
       </c>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B71" s="111" t="s">
+      <c r="B71" s="113" t="s">
         <v>104</v>
       </c>
       <c r="C71" s="58">
@@ -35413,7 +35413,7 @@
       </c>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="112"/>
+      <c r="B72" s="114"/>
       <c r="C72" s="67">
         <v>0.45700000000000002</v>
       </c>
@@ -35455,7 +35455,7 @@
       </c>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="112"/>
+      <c r="B73" s="114"/>
       <c r="C73" s="75">
         <v>0.66700000000000004</v>
       </c>
@@ -35497,7 +35497,7 @@
       </c>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="112"/>
+      <c r="B74" s="114"/>
       <c r="C74" s="69">
         <v>0.54400000000000004</v>
       </c>
@@ -35539,7 +35539,7 @@
       </c>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="113"/>
+      <c r="B75" s="115"/>
       <c r="C75" s="81">
         <v>0.61599999999999999</v>
       </c>
@@ -35581,7 +35581,7 @@
       </c>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B76" s="111" t="s">
+      <c r="B76" s="113" t="s">
         <v>117</v>
       </c>
       <c r="C76" s="96">
@@ -35625,7 +35625,7 @@
       </c>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B77" s="112"/>
+      <c r="B77" s="114"/>
       <c r="C77" s="74">
         <v>0.442</v>
       </c>
@@ -35667,7 +35667,7 @@
       </c>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="112"/>
+      <c r="B78" s="114"/>
       <c r="C78" s="74">
         <v>0.64700000000000002</v>
       </c>
@@ -35709,7 +35709,7 @@
       </c>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="112"/>
+      <c r="B79" s="114"/>
       <c r="C79" s="74">
         <v>0.53200000000000003</v>
       </c>
@@ -35751,7 +35751,7 @@
       </c>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="113"/>
+      <c r="B80" s="115"/>
       <c r="C80" s="81">
         <v>0.61799999999999999</v>
       </c>
@@ -38220,7 +38220,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="111" t="s">
+      <c r="B41" s="113" t="s">
         <v>25</v>
       </c>
       <c r="C41" s="60">
@@ -38264,7 +38264,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="112"/>
+      <c r="B42" s="114"/>
       <c r="C42" s="67">
         <v>0.46600000000000003</v>
       </c>
@@ -38306,7 +38306,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="112"/>
+      <c r="B43" s="114"/>
       <c r="C43" s="69">
         <v>0.71</v>
       </c>
@@ -38348,7 +38348,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="112"/>
+      <c r="B44" s="114"/>
       <c r="C44" s="69">
         <v>0.55000000000000004</v>
       </c>
@@ -38390,7 +38390,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="113"/>
+      <c r="B45" s="115"/>
       <c r="C45" s="78">
         <v>0.504</v>
       </c>
@@ -38432,7 +38432,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="111" t="s">
+      <c r="B46" s="113" t="s">
         <v>39</v>
       </c>
       <c r="C46" s="59">
@@ -38476,7 +38476,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="112"/>
+      <c r="B47" s="114"/>
       <c r="C47" s="68">
         <v>0.47299999999999998</v>
       </c>
@@ -38518,7 +38518,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="112"/>
+      <c r="B48" s="114"/>
       <c r="C48" s="71">
         <v>0.73399999999999999</v>
       </c>
@@ -38560,7 +38560,7 @@
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="112"/>
+      <c r="B49" s="114"/>
       <c r="C49" s="71">
         <v>0.55800000000000005</v>
       </c>
@@ -38602,7 +38602,7 @@
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="113"/>
+      <c r="B50" s="115"/>
       <c r="C50" s="88">
         <v>0.47</v>
       </c>
@@ -38644,7 +38644,7 @@
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="111" t="s">
+      <c r="B51" s="113" t="s">
         <v>52</v>
       </c>
       <c r="C51" s="65">
@@ -38688,7 +38688,7 @@
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B52" s="112"/>
+      <c r="B52" s="114"/>
       <c r="C52" s="85">
         <v>0.505</v>
       </c>
@@ -38730,7 +38730,7 @@
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="112"/>
+      <c r="B53" s="114"/>
       <c r="C53" s="87">
         <v>0.80800000000000005</v>
       </c>
@@ -38772,7 +38772,7 @@
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="112"/>
+      <c r="B54" s="114"/>
       <c r="C54" s="73">
         <v>0.56899999999999995</v>
       </c>
@@ -38814,7 +38814,7 @@
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="113"/>
+      <c r="B55" s="115"/>
       <c r="C55" s="89">
         <v>0.29199999999999998</v>
       </c>
@@ -38856,7 +38856,7 @@
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="111" t="s">
+      <c r="B56" s="113" t="s">
         <v>65</v>
       </c>
       <c r="C56" s="83">
@@ -38900,7 +38900,7 @@
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="112"/>
+      <c r="B57" s="114"/>
       <c r="C57" s="71">
         <v>0.47899999999999998</v>
       </c>
@@ -38942,7 +38942,7 @@
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="112"/>
+      <c r="B58" s="114"/>
       <c r="C58" s="67">
         <v>0.69199999999999995</v>
       </c>
@@ -38984,7 +38984,7 @@
       </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="112"/>
+      <c r="B59" s="114"/>
       <c r="C59" s="70">
         <v>0.56399999999999995</v>
       </c>
@@ -39026,7 +39026,7 @@
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="113"/>
+      <c r="B60" s="115"/>
       <c r="C60" s="81">
         <v>0.63200000000000001</v>
       </c>
@@ -39068,7 +39068,7 @@
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="111" t="s">
+      <c r="B61" s="113" t="s">
         <v>78</v>
       </c>
       <c r="C61" s="58">
@@ -39112,7 +39112,7 @@
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="112"/>
+      <c r="B62" s="114"/>
       <c r="C62" s="67">
         <v>0.46500000000000002</v>
       </c>
@@ -39154,7 +39154,7 @@
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="112"/>
+      <c r="B63" s="114"/>
       <c r="C63" s="66">
         <v>0.68100000000000005</v>
       </c>
@@ -39196,7 +39196,7 @@
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="112"/>
+      <c r="B64" s="114"/>
       <c r="C64" s="71">
         <v>0.55600000000000005</v>
       </c>
@@ -39238,7 +39238,7 @@
       </c>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B65" s="113"/>
+      <c r="B65" s="115"/>
       <c r="C65" s="81">
         <v>0.63300000000000001</v>
       </c>
@@ -39280,7 +39280,7 @@
       </c>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B66" s="111" t="s">
+      <c r="B66" s="113" t="s">
         <v>91</v>
       </c>
       <c r="C66" s="62">
@@ -39324,7 +39324,7 @@
       </c>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B67" s="112"/>
+      <c r="B67" s="114"/>
       <c r="C67" s="71">
         <v>0.48299999999999998</v>
       </c>
@@ -39366,7 +39366,7 @@
       </c>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="112"/>
+      <c r="B68" s="114"/>
       <c r="C68" s="67">
         <v>0.69199999999999995</v>
       </c>
@@ -39408,7 +39408,7 @@
       </c>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="112"/>
+      <c r="B69" s="114"/>
       <c r="C69" s="70">
         <v>0.56499999999999995</v>
       </c>
@@ -39450,7 +39450,7 @@
       </c>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="113"/>
+      <c r="B70" s="115"/>
       <c r="C70" s="81">
         <v>0.63400000000000001</v>
       </c>
@@ -39492,7 +39492,7 @@
       </c>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B71" s="111" t="s">
+      <c r="B71" s="113" t="s">
         <v>104</v>
       </c>
       <c r="C71" s="59">
@@ -39536,7 +39536,7 @@
       </c>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="112"/>
+      <c r="B72" s="114"/>
       <c r="C72" s="67">
         <v>0.46500000000000002</v>
       </c>
@@ -39578,7 +39578,7 @@
       </c>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="112"/>
+      <c r="B73" s="114"/>
       <c r="C73" s="75">
         <v>0.67500000000000004</v>
       </c>
@@ -39620,7 +39620,7 @@
       </c>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="112"/>
+      <c r="B74" s="114"/>
       <c r="C74" s="69">
         <v>0.55000000000000004</v>
       </c>
@@ -39662,7 +39662,7 @@
       </c>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="113"/>
+      <c r="B75" s="115"/>
       <c r="C75" s="80">
         <v>0.621</v>
       </c>
@@ -39704,7 +39704,7 @@
       </c>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B76" s="111" t="s">
+      <c r="B76" s="113" t="s">
         <v>117</v>
       </c>
       <c r="C76" s="60">
@@ -39748,7 +39748,7 @@
       </c>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B77" s="112"/>
+      <c r="B77" s="114"/>
       <c r="C77" s="67">
         <v>0.46200000000000002</v>
       </c>
@@ -39790,7 +39790,7 @@
       </c>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="112"/>
+      <c r="B78" s="114"/>
       <c r="C78" s="75">
         <v>0.67600000000000005</v>
       </c>
@@ -39832,7 +39832,7 @@
       </c>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="112"/>
+      <c r="B79" s="114"/>
       <c r="C79" s="68">
         <v>0.55200000000000005</v>
       </c>
@@ -39874,7 +39874,7 @@
       </c>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="113"/>
+      <c r="B80" s="115"/>
       <c r="C80" s="81">
         <v>0.63</v>
       </c>
@@ -42343,7 +42343,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="111" t="s">
+      <c r="B41" s="113" t="s">
         <v>25</v>
       </c>
       <c r="C41" s="64">
@@ -42387,7 +42387,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="112"/>
+      <c r="B42" s="114"/>
       <c r="C42" s="73">
         <v>0.47099999999999997</v>
       </c>
@@ -42429,7 +42429,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="112"/>
+      <c r="B43" s="114"/>
       <c r="C43" s="72">
         <v>0.69399999999999995</v>
       </c>
@@ -42471,7 +42471,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="112"/>
+      <c r="B44" s="114"/>
       <c r="C44" s="73">
         <v>0.55700000000000005</v>
       </c>
@@ -42513,7 +42513,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="113"/>
+      <c r="B45" s="115"/>
       <c r="C45" s="77">
         <v>0.58799999999999997</v>
       </c>
@@ -42555,7 +42555,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="111" t="s">
+      <c r="B46" s="113" t="s">
         <v>39</v>
       </c>
       <c r="C46" s="83">
@@ -42599,7 +42599,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="112"/>
+      <c r="B47" s="114"/>
       <c r="C47" s="71">
         <v>0.45300000000000001</v>
       </c>
@@ -42641,7 +42641,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="112"/>
+      <c r="B48" s="114"/>
       <c r="C48" s="68">
         <v>0.66800000000000004</v>
       </c>
@@ -42683,7 +42683,7 @@
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="112"/>
+      <c r="B49" s="114"/>
       <c r="C49" s="70">
         <v>0.54700000000000004</v>
       </c>
@@ -42725,7 +42725,7 @@
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="113"/>
+      <c r="B50" s="115"/>
       <c r="C50" s="80">
         <v>0.627</v>
       </c>
@@ -42767,7 +42767,7 @@
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="111" t="s">
+      <c r="B51" s="113" t="s">
         <v>52</v>
       </c>
       <c r="C51" s="62">
@@ -42811,7 +42811,7 @@
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B52" s="112"/>
+      <c r="B52" s="114"/>
       <c r="C52" s="70">
         <v>0.46600000000000003</v>
       </c>
@@ -42853,7 +42853,7 @@
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="112"/>
+      <c r="B53" s="114"/>
       <c r="C53" s="72">
         <v>0.70799999999999996</v>
       </c>
@@ -42895,7 +42895,7 @@
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="112"/>
+      <c r="B54" s="114"/>
       <c r="C54" s="73">
         <v>0.55400000000000005</v>
       </c>
@@ -42937,7 +42937,7 @@
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="113"/>
+      <c r="B55" s="115"/>
       <c r="C55" s="76">
         <v>0.52900000000000003</v>
       </c>
@@ -42979,7 +42979,7 @@
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="111" t="s">
+      <c r="B56" s="113" t="s">
         <v>65</v>
       </c>
       <c r="C56" s="61">
@@ -43023,7 +43023,7 @@
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="112"/>
+      <c r="B57" s="114"/>
       <c r="C57" s="84">
         <v>0.48</v>
       </c>
@@ -43065,7 +43065,7 @@
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="112"/>
+      <c r="B58" s="114"/>
       <c r="C58" s="85">
         <v>0.75600000000000001</v>
       </c>
@@ -43107,7 +43107,7 @@
       </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="112"/>
+      <c r="B59" s="114"/>
       <c r="C59" s="84">
         <v>0.55900000000000005</v>
       </c>
@@ -43149,7 +43149,7 @@
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="113"/>
+      <c r="B60" s="115"/>
       <c r="C60" s="93">
         <v>0.40300000000000002</v>
       </c>
@@ -43191,7 +43191,7 @@
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="111" t="s">
+      <c r="B61" s="113" t="s">
         <v>78</v>
       </c>
       <c r="C61" s="90">
@@ -43235,7 +43235,7 @@
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="112"/>
+      <c r="B62" s="114"/>
       <c r="C62" s="86">
         <v>0.5</v>
       </c>
@@ -43277,7 +43277,7 @@
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="112"/>
+      <c r="B63" s="114"/>
       <c r="C63" s="86">
         <v>0.78200000000000003</v>
       </c>
@@ -43319,7 +43319,7 @@
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="112"/>
+      <c r="B64" s="114"/>
       <c r="C64" s="86">
         <v>0.57499999999999996</v>
       </c>
@@ -43361,7 +43361,7 @@
       </c>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B65" s="113"/>
+      <c r="B65" s="115"/>
       <c r="C65" s="93">
         <v>0.39500000000000002</v>
       </c>
@@ -43403,7 +43403,7 @@
       </c>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B66" s="111" t="s">
+      <c r="B66" s="113" t="s">
         <v>91</v>
       </c>
       <c r="C66" s="96">
@@ -43447,7 +43447,7 @@
       </c>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B67" s="112"/>
+      <c r="B67" s="114"/>
       <c r="C67" s="75">
         <v>0.41199999999999998</v>
       </c>
@@ -43489,7 +43489,7 @@
       </c>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="112"/>
+      <c r="B68" s="114"/>
       <c r="C68" s="75">
         <v>0.60799999999999998</v>
       </c>
@@ -43531,7 +43531,7 @@
       </c>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="112"/>
+      <c r="B69" s="114"/>
       <c r="C69" s="66">
         <v>0.51300000000000001</v>
       </c>
@@ -43573,7 +43573,7 @@
       </c>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="113"/>
+      <c r="B70" s="115"/>
       <c r="C70" s="81">
         <v>0.65400000000000003</v>
       </c>
@@ -43615,7 +43615,7 @@
       </c>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B71" s="111" t="s">
+      <c r="B71" s="113" t="s">
         <v>104</v>
       </c>
       <c r="C71" s="96">
@@ -43659,7 +43659,7 @@
       </c>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="112"/>
+      <c r="B72" s="114"/>
       <c r="C72" s="75">
         <v>0.40899999999999997</v>
       </c>
@@ -43701,7 +43701,7 @@
       </c>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="112"/>
+      <c r="B73" s="114"/>
       <c r="C73" s="74">
         <v>0.60099999999999998</v>
       </c>
@@ -43743,7 +43743,7 @@
       </c>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="112"/>
+      <c r="B74" s="114"/>
       <c r="C74" s="75">
         <v>0.50700000000000001</v>
       </c>
@@ -43785,7 +43785,7 @@
       </c>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="113"/>
+      <c r="B75" s="115"/>
       <c r="C75" s="81">
         <v>0.64700000000000002</v>
       </c>
@@ -43827,7 +43827,7 @@
       </c>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B76" s="111" t="s">
+      <c r="B76" s="113" t="s">
         <v>117</v>
       </c>
       <c r="C76" s="94">
@@ -43871,7 +43871,7 @@
       </c>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B77" s="112"/>
+      <c r="B77" s="114"/>
       <c r="C77" s="74">
         <v>0.4</v>
       </c>
@@ -43913,7 +43913,7 @@
       </c>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="112"/>
+      <c r="B78" s="114"/>
       <c r="C78" s="74">
         <v>0.58799999999999997</v>
       </c>
@@ -43955,7 +43955,7 @@
       </c>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="112"/>
+      <c r="B79" s="114"/>
       <c r="C79" s="74">
         <v>0.496</v>
       </c>
@@ -43997,7 +43997,7 @@
       </c>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="113"/>
+      <c r="B80" s="115"/>
       <c r="C80" s="80">
         <v>0.63200000000000001</v>
       </c>
@@ -46466,7 +46466,7 @@
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="111" t="s">
+      <c r="B41" s="113" t="s">
         <v>25</v>
       </c>
       <c r="C41" s="64">
@@ -46510,7 +46510,7 @@
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="112"/>
+      <c r="B42" s="114"/>
       <c r="C42" s="73">
         <v>0.46899999999999997</v>
       </c>
@@ -46552,7 +46552,7 @@
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B43" s="112"/>
+      <c r="B43" s="114"/>
       <c r="C43" s="68">
         <v>0.69</v>
       </c>
@@ -46594,7 +46594,7 @@
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B44" s="112"/>
+      <c r="B44" s="114"/>
       <c r="C44" s="70">
         <v>0.55100000000000005</v>
       </c>
@@ -46636,7 +46636,7 @@
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B45" s="113"/>
+      <c r="B45" s="115"/>
       <c r="C45" s="79">
         <v>0.57699999999999996</v>
       </c>
@@ -46678,7 +46678,7 @@
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B46" s="111" t="s">
+      <c r="B46" s="113" t="s">
         <v>39</v>
       </c>
       <c r="C46" s="64">
@@ -46722,7 +46722,7 @@
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B47" s="112"/>
+      <c r="B47" s="114"/>
       <c r="C47" s="73">
         <v>0.47</v>
       </c>
@@ -46764,7 +46764,7 @@
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B48" s="112"/>
+      <c r="B48" s="114"/>
       <c r="C48" s="68">
         <v>0.68300000000000005</v>
       </c>
@@ -46806,7 +46806,7 @@
       </c>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B49" s="112"/>
+      <c r="B49" s="114"/>
       <c r="C49" s="84">
         <v>0.55600000000000005</v>
       </c>
@@ -46848,7 +46848,7 @@
       </c>
     </row>
     <row r="50" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B50" s="113"/>
+      <c r="B50" s="115"/>
       <c r="C50" s="80">
         <v>0.627</v>
       </c>
@@ -46890,7 +46890,7 @@
       </c>
     </row>
     <row r="51" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B51" s="111" t="s">
+      <c r="B51" s="113" t="s">
         <v>52</v>
       </c>
       <c r="C51" s="61">
@@ -46934,7 +46934,7 @@
       </c>
     </row>
     <row r="52" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B52" s="112"/>
+      <c r="B52" s="114"/>
       <c r="C52" s="85">
         <v>0.47799999999999998</v>
       </c>
@@ -46976,7 +46976,7 @@
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B53" s="112"/>
+      <c r="B53" s="114"/>
       <c r="C53" s="70">
         <v>0.72299999999999998</v>
       </c>
@@ -47018,7 +47018,7 @@
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B54" s="112"/>
+      <c r="B54" s="114"/>
       <c r="C54" s="85">
         <v>0.56100000000000005</v>
       </c>
@@ -47060,7 +47060,7 @@
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B55" s="113"/>
+      <c r="B55" s="115"/>
       <c r="C55" s="78">
         <v>0.51600000000000001</v>
       </c>
@@ -47102,7 +47102,7 @@
       </c>
     </row>
     <row r="56" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B56" s="111" t="s">
+      <c r="B56" s="113" t="s">
         <v>65</v>
       </c>
       <c r="C56" s="64">
@@ -47146,7 +47146,7 @@
       </c>
     </row>
     <row r="57" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B57" s="112"/>
+      <c r="B57" s="114"/>
       <c r="C57" s="84">
         <v>0.47599999999999998</v>
       </c>
@@ -47188,7 +47188,7 @@
       </c>
     </row>
     <row r="58" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B58" s="112"/>
+      <c r="B58" s="114"/>
       <c r="C58" s="84">
         <v>0.747</v>
       </c>
@@ -47230,7 +47230,7 @@
       </c>
     </row>
     <row r="59" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B59" s="112"/>
+      <c r="B59" s="114"/>
       <c r="C59" s="84">
         <v>0.55600000000000005</v>
       </c>
@@ -47272,7 +47272,7 @@
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B60" s="113"/>
+      <c r="B60" s="115"/>
       <c r="C60" s="93">
         <v>0.41599999999999998</v>
       </c>
@@ -47314,7 +47314,7 @@
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B61" s="111" t="s">
+      <c r="B61" s="113" t="s">
         <v>78</v>
       </c>
       <c r="C61" s="91">
@@ -47358,7 +47358,7 @@
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B62" s="112"/>
+      <c r="B62" s="114"/>
       <c r="C62" s="86">
         <v>0.48699999999999999</v>
       </c>
@@ -47400,7 +47400,7 @@
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B63" s="112"/>
+      <c r="B63" s="114"/>
       <c r="C63" s="85">
         <v>0.76</v>
       </c>
@@ -47442,7 +47442,7 @@
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B64" s="112"/>
+      <c r="B64" s="114"/>
       <c r="C64" s="86">
         <v>0.56499999999999995</v>
       </c>
@@ -47484,7 +47484,7 @@
       </c>
     </row>
     <row r="65" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B65" s="113"/>
+      <c r="B65" s="115"/>
       <c r="C65" s="95">
         <v>0.42</v>
       </c>
@@ -47526,7 +47526,7 @@
       </c>
     </row>
     <row r="66" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B66" s="111" t="s">
+      <c r="B66" s="113" t="s">
         <v>91</v>
       </c>
       <c r="C66" s="96">
@@ -47570,7 +47570,7 @@
       </c>
     </row>
     <row r="67" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B67" s="112"/>
+      <c r="B67" s="114"/>
       <c r="C67" s="66">
         <v>0.42799999999999999</v>
       </c>
@@ -47612,7 +47612,7 @@
       </c>
     </row>
     <row r="68" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B68" s="112"/>
+      <c r="B68" s="114"/>
       <c r="C68" s="69">
         <v>0.67600000000000005</v>
       </c>
@@ -47654,7 +47654,7 @@
       </c>
     </row>
     <row r="69" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="112"/>
+      <c r="B69" s="114"/>
       <c r="C69" s="72">
         <v>0.54500000000000004</v>
       </c>
@@ -47696,7 +47696,7 @@
       </c>
     </row>
     <row r="70" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B70" s="113"/>
+      <c r="B70" s="115"/>
       <c r="C70" s="78">
         <v>0.51100000000000001</v>
       </c>
@@ -47738,7 +47738,7 @@
       </c>
     </row>
     <row r="71" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B71" s="111" t="s">
+      <c r="B71" s="113" t="s">
         <v>104</v>
       </c>
       <c r="C71" s="96">
@@ -47782,7 +47782,7 @@
       </c>
     </row>
     <row r="72" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="112"/>
+      <c r="B72" s="114"/>
       <c r="C72" s="66">
         <v>0.42799999999999999</v>
       </c>
@@ -47824,7 +47824,7 @@
       </c>
     </row>
     <row r="73" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="112"/>
+      <c r="B73" s="114"/>
       <c r="C73" s="69">
         <v>0.67500000000000004</v>
       </c>
@@ -47866,7 +47866,7 @@
       </c>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="112"/>
+      <c r="B74" s="114"/>
       <c r="C74" s="72">
         <v>0.54400000000000004</v>
       </c>
@@ -47908,7 +47908,7 @@
       </c>
     </row>
     <row r="75" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B75" s="113"/>
+      <c r="B75" s="115"/>
       <c r="C75" s="78">
         <v>0.51</v>
       </c>
@@ -47950,7 +47950,7 @@
       </c>
     </row>
     <row r="76" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B76" s="111" t="s">
+      <c r="B76" s="113" t="s">
         <v>117</v>
       </c>
       <c r="C76" s="96">
@@ -47994,7 +47994,7 @@
       </c>
     </row>
     <row r="77" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B77" s="112"/>
+      <c r="B77" s="114"/>
       <c r="C77" s="66">
         <v>0.42899999999999999</v>
       </c>
@@ -48036,7 +48036,7 @@
       </c>
     </row>
     <row r="78" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="112"/>
+      <c r="B78" s="114"/>
       <c r="C78" s="69">
         <v>0.67800000000000005</v>
       </c>
@@ -48078,7 +48078,7 @@
       </c>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="112"/>
+      <c r="B79" s="114"/>
       <c r="C79" s="72">
         <v>0.54700000000000004</v>
       </c>
@@ -48120,7 +48120,7 @@
       </c>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="113"/>
+      <c r="B80" s="115"/>
       <c r="C80" s="78">
         <v>0.51</v>
       </c>

</xml_diff>

<commit_message>
HBS size Crystal str vs AF, F- calibration data, Mono vs Difluoroacetate plot
</commit_message>
<xml_diff>
--- a/Dehalogenation_colorimetric_assays/Fluoride Library screening 1 to 3 diluted.xlsx
+++ b/Dehalogenation_colorimetric_assays/Fluoride Library screening 1 to 3 diluted.xlsx
@@ -3363,8 +3363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BE118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A82" sqref="A82"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -17672,8 +17672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:O72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T37" sqref="T37"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37:H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>